<commit_message>
moved to excelize, avoid windows
</commit_message>
<xml_diff>
--- a/SCRIPTS/SGSN_template.xlsx
+++ b/SCRIPTS/SGSN_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -17,10 +17,56 @@
     <sheet name="3G" sheetId="13" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_aa" localSheetId="2">OFFSET('3G'!$AA$2,0,0,COUNTA('3G'!$AA:$AA)-1)</definedName>
+    <definedName name="_ab" localSheetId="2">OFFSET('3G'!$AB$2,0,0,COUNTA('3G'!$AB:$AB)-1)</definedName>
+    <definedName name="_ac" localSheetId="1">OFFSET('2G'!$AC$2,0,0,COUNTA('2G'!$AC:$AC)-1)</definedName>
+    <definedName name="_ac" localSheetId="2">OFFSET('3G'!$AC$2,0,0,COUNTA('3G'!$AC:$AC)-1)</definedName>
+    <definedName name="_ad" localSheetId="1">OFFSET('2G'!$AD$2,0,0,COUNTA('2G'!$AD:$AD)-1)</definedName>
+    <definedName name="_ad" localSheetId="2">OFFSET('3G'!$AD$2,0,0,COUNTA('3G'!$AD:$AD)-1)</definedName>
+    <definedName name="_ae" localSheetId="1">OFFSET('2G'!$AE$2,0,0,COUNTA('2G'!$AE:$AE)-1)</definedName>
+    <definedName name="_ae" localSheetId="2">OFFSET('3G'!$AE$2,0,0,COUNTA('3G'!$AE:$AE)-1)</definedName>
+    <definedName name="_af" localSheetId="1">OFFSET('2G'!$AF$2,0,0,COUNTA('2G'!$AF:$AF)-1)</definedName>
+    <definedName name="_af" localSheetId="2">OFFSET('3G'!$AF$2,0,0,COUNTA('3G'!$AF:$AF)-1)</definedName>
+    <definedName name="_ah" localSheetId="1">OFFSET('2G'!$AH$2,0,0,COUNTA('2G'!$AH:$AH)-1)</definedName>
+    <definedName name="_ai" localSheetId="1">OFFSET('2G'!$AI$2,0,0,COUNTA('2G'!$AI:$AI)-1)</definedName>
+    <definedName name="_aj" localSheetId="1">OFFSET('2G'!$AJ$2,0,0,COUNTA('2G'!$AJ:$AJ)-1)</definedName>
+    <definedName name="_ak" localSheetId="1">OFFSET('2G'!$AK$2,0,0,COUNTA('2G'!$AK:$AK)-1)</definedName>
+    <definedName name="_al" localSheetId="1">OFFSET('2G'!$AL$2,0,0,COUNTA('2G'!$AL:$AL)-1)</definedName>
+    <definedName name="_am" localSheetId="2">OFFSET('3G'!$AM$2,0,0,COUNTA('3G'!$AM:$AM)-1)</definedName>
+    <definedName name="_an" localSheetId="2">OFFSET('3G'!$AN$2,0,0,COUNTA('3G'!$AN:$AN)-1)</definedName>
+    <definedName name="_ao" localSheetId="2">OFFSET('3G'!$AO$2,0,0,COUNTA('3G'!$AO:$AO)-1)</definedName>
+    <definedName name="_ap" localSheetId="2">OFFSET('3G'!$AP$2,0,0,COUNTA('3G'!$AP:$AP)-1)</definedName>
+    <definedName name="_aq" localSheetId="2">OFFSET('3G'!$AQ$2,0,0,COUNTA('3G'!$AQ:$AQ)-1)</definedName>
+    <definedName name="_ar" localSheetId="2">OFFSET('3G'!$AR$2,0,0,COUNTA('3G'!$AR:$AR)-1)</definedName>
+    <definedName name="_c" localSheetId="1">OFFSET('2G'!$C$2,0,0,COUNTA('2G'!$C:$C)-1)</definedName>
+    <definedName name="_c" localSheetId="2">OFFSET('3G'!$C$2,0,0,COUNTA('3G'!$C:$C)-1)</definedName>
+    <definedName name="_d" localSheetId="2">OFFSET('3G'!$D$2,0,0,COUNTA('3G'!$D:$D)-1)</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'3G'!$A$1:$AH$2</definedName>
+    <definedName name="_g" localSheetId="1">OFFSET('2G'!$G$2,0,0,COUNTA('2G'!$G:$G)-1)</definedName>
+    <definedName name="_g" localSheetId="2">OFFSET('3G'!$G$2,0,0,COUNTA('3G'!$G:$G)-1)</definedName>
+    <definedName name="_h" localSheetId="1">OFFSET('2G'!$H$2,0,0,COUNTA('2G'!$H:$H)-1)</definedName>
+    <definedName name="_h" localSheetId="2">OFFSET('3G'!$H$2,0,0,COUNTA('3G'!$H:$H)-1)</definedName>
+    <definedName name="_i" localSheetId="1">OFFSET('2G'!$I$2,0,0,COUNTA('2G'!$I:$I)-1)</definedName>
+    <definedName name="_i" localSheetId="2">OFFSET('3G'!$I$2,0,0,COUNTA('3G'!$I:$I)-1)</definedName>
+    <definedName name="_j" localSheetId="1">OFFSET('2G'!$J$2,0,0,COUNTA('2G'!$J:$J)-1)</definedName>
+    <definedName name="_j" localSheetId="2">OFFSET('3G'!$J$2,0,0,COUNTA('3G'!$J:$J)-1)</definedName>
+    <definedName name="_k" localSheetId="1">OFFSET('2G'!$K$2,0,0,COUNTA('2G'!$K:$K)-1)</definedName>
+    <definedName name="_k" localSheetId="2">OFFSET('3G'!$K$2,0,0,COUNTA('3G'!$K:$K)-1)</definedName>
+    <definedName name="_l" localSheetId="1">OFFSET('2G'!$L$2,0,0,COUNTA('2G'!$L:$L)-1)</definedName>
+    <definedName name="_l" localSheetId="2">OFFSET('3G'!$L$2,0,0,COUNTA('3G'!$L:$L)-1)</definedName>
+    <definedName name="_o" localSheetId="1">OFFSET('2G'!$O$2,0,0,COUNTA('2G'!$O:$O)-1)</definedName>
+    <definedName name="_s" localSheetId="2">OFFSET('3G'!$S$2,0,0,COUNTA('3G'!$S:$S)-1)</definedName>
+    <definedName name="_w" localSheetId="1">OFFSET('2G'!$W$2,0,0,COUNTA('2G'!$W:$W)-1)</definedName>
+    <definedName name="_x" localSheetId="1">OFFSET('2G'!$X$2,0,0,COUNTA('2G'!$X:$X)-1)</definedName>
+    <definedName name="_x" localSheetId="2">OFFSET('3G'!$X$2,0,0,COUNTA('3G'!$X:$X)-1)</definedName>
+    <definedName name="_y" localSheetId="1">OFFSET('2G'!$Y$2,0,0,COUNTA('2G'!$Y:$Y)-1)</definedName>
+    <definedName name="_y" localSheetId="2">OFFSET('3G'!$Y$2,0,0,COUNTA('3G'!$Y:$Y)-1)</definedName>
+    <definedName name="_z" localSheetId="1">OFFSET('2G'!$Z$2,0,0,COUNTA('2G'!$Z:$Z)-1)</definedName>
+    <definedName name="_z" localSheetId="2">OFFSET('3G'!$Z$2,0,0,COUNTA('3G'!$Z:$Z)-1)</definedName>
+    <definedName name="Time" localSheetId="1">OFFSET('2G'!$B$2,0,0,COUNTA('2G'!$B:$B)-1)</definedName>
+    <definedName name="Time" localSheetId="2">OFFSET('3G'!$B$2,0,0,COUNTA('3G'!$B:$B)-1)</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -268,9 +314,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,7 +468,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,28 +648,25 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -737,34 +777,99 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="8"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -790,19 +895,29 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -851,7 +966,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="1">
     <dxf>
       <font>
         <condense val="0"/>
@@ -863,199 +978,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1107,20 +1029,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$C$2:$C$2</c:f>
+              <c:f>'2G'!_c</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1150,7 +1071,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1282,20 +1203,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AO$2:$AO$2</c:f>
+              <c:f>'3G'!_ao</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1325,7 +1245,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1357,7 +1277,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1463,20 +1383,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$G$2:$G$2</c:f>
+              <c:f>'3G'!_g</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1505,20 +1424,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$H$2:$H$2</c:f>
+              <c:f>'3G'!_h</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1547,20 +1465,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$I$2:$I$2</c:f>
+              <c:f>'3G'!_i</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1589,20 +1506,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$J$2:$J$2</c:f>
+              <c:f>'3G'!_j</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1631,20 +1547,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$K$2:$K$2</c:f>
+              <c:f>'3G'!_k</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1673,20 +1588,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$L$2:$L$2</c:f>
+              <c:f>'3G'!_l</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1716,7 +1630,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1852,20 +1766,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$X$2:$X$2</c:f>
+              <c:f>'3G'!_x</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1894,20 +1807,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$Y$2:$Y$2</c:f>
+              <c:f>'3G'!_y</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1936,20 +1848,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$Z$2:$Z$2</c:f>
+              <c:f>'3G'!_z</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1978,20 +1889,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AA$2:$AA$2</c:f>
+              <c:f>'3G'!_aa</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2020,20 +1930,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AB$2:$AB$2</c:f>
+              <c:f>'3G'!_ab</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2062,20 +1971,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AC$2:$AC$2</c:f>
+              <c:f>'3G'!_ac</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2104,20 +2012,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AD$2:$AD$2</c:f>
+              <c:f>'3G'!_ad</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2146,20 +2053,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AE$2:$AE$2</c:f>
+              <c:f>'3G'!_ae</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2188,20 +2094,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AF$2:$AF$2</c:f>
+              <c:f>'3G'!_af</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2231,7 +2136,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2367,20 +2272,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$G$2:$G$2</c:f>
+              <c:f>'2G'!_g</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2409,20 +2313,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$H$2:$H$2</c:f>
+              <c:f>'2G'!_h</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2451,20 +2354,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$I$2:$I$2</c:f>
+              <c:f>'2G'!_i</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2493,20 +2395,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$J$2:$J$2</c:f>
+              <c:f>'2G'!_j</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2540,20 +2441,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$K$2:$K$2</c:f>
+              <c:f>'2G'!_k</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2582,20 +2482,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$L$2:$L$2</c:f>
+              <c:f>'2G'!_l</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2624,20 +2523,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$O$2:$O$2</c:f>
+              <c:f>'2G'!_o</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2667,7 +2565,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2803,20 +2701,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AP$2:$AP$2</c:f>
+              <c:f>'3G'!_ap</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2845,20 +2742,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AQ$2:$AQ$2</c:f>
+              <c:f>'3G'!_aq</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2887,20 +2783,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AR$2:$AR$2</c:f>
+              <c:f>'3G'!_ar</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2930,7 +2825,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3043,20 +2938,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$Z$2:$Z$2</c:f>
+              <c:f>'2G'!_z</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3086,7 +2980,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3230,20 +3124,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$AH$2:$AH$2</c:f>
+              <c:f>'2G'!_ah</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3272,20 +3165,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$AI$2:$AI$2</c:f>
+              <c:f>'2G'!_ai</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3315,7 +3207,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3358,7 +3250,7 @@
             </a:ln>
           </c:spPr>
         </c:minorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3460,20 +3352,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$AJ$2:$AJ$2</c:f>
+              <c:f>'2G'!_aj</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3503,7 +3394,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3535,7 +3426,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3641,20 +3532,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$W$2:$W$2</c:f>
+              <c:f>'2G'!_w</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3683,20 +3573,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$X$2:$X$2</c:f>
+              <c:f>'2G'!_x</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3725,20 +3614,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$Y$2:$Y$2</c:f>
+              <c:f>'2G'!_y</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3766,12 +3654,20 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$AC$2:$AC$2</c:f>
+              <c:f>'2G'!_ac</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3799,12 +3695,20 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$AD$2:$AD$2</c:f>
+              <c:f>'2G'!_ad</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3832,12 +3736,20 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$AE$2:$AE$2</c:f>
+              <c:f>'2G'!_ae</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3865,12 +3777,20 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$AF$2:$AF$2</c:f>
+              <c:f>'2G'!_af</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3900,7 +3820,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4036,20 +3956,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$AK$2:$AK$2</c:f>
+              <c:f>'2G'!_ak</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4078,20 +3997,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'2G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'2G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2G'!$AL$2:$AL$2</c:f>
+              <c:f>'2G'!_al</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4121,7 +4039,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4257,20 +4175,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$C$2:$C$2</c:f>
+              <c:f>'3G'!_c</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4319,32 +4236,31 @@
                   <c:symbol val="none"/>
                 </c:marker>
                 <c:cat>
-                  <c:numRef>
+                  <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'3G'!$B$2:$B$2</c15:sqref>
+                          <c15:sqref>'3G'!Time</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>h:mm</c:formatCode>
-                      <c:ptCount val="1"/>
-                    </c:numCache>
-                  </c:numRef>
+                  </c:multiLvlStrRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'3G'!$D$2:$D$2</c15:sqref>
+                          <c15:sqref>'3G'!_d</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4366,7 +4282,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4502,20 +4418,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AM$2:$AM$2</c:f>
+              <c:f>'3G'!_am</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4543,12 +4458,20 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$AN$2:$AN$2</c:f>
+              <c:f>'3G'!_an</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4578,7 +4501,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4609,7 +4532,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4710,20 +4633,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>'3G'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>'3G'!Time</c:f>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3G'!$S$2:$S$2</c:f>
+              <c:f>'3G'!_s</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4753,7 +4675,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5386,128 +5308,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:AL2" insertRow="1" totalsRowShown="0" headerRowDxfId="18">
-  <autoFilter ref="A1:AL2"/>
-  <tableColumns count="38">
-    <tableColumn id="1" name="Date" dataDxfId="17"/>
-    <tableColumn id="2" name="Time" dataDxfId="16"/>
-    <tableColumn id="3" name="VS.Gmm_AveNbrOfAttachedSub_G"/>
-    <tableColumn id="4" name="VS.Gmm_MaxNbrOfAttachedSub_G"/>
-    <tableColumn id="5" name="VS.Gmm_attGprsAttach_G"/>
-    <tableColumn id="6" name="VS.Gmm_succGprsAttach_G"/>
-    <tableColumn id="7" name="VS.Gmm_rejGprsAttachSgsnInternal_G"/>
-    <tableColumn id="8" name="VS.Gmm_rejGprsAttachProtocolError_G"/>
-    <tableColumn id="9" name="VS.Gmm_rejGprsAttachNetworkFailure_G"/>
-    <tableColumn id="10" name="VS.Gmm_attGprsAttachRandomCollision_G"/>
-    <tableColumn id="11" name="VS.Gmm_rejGprsAttachNotAllowed_G"/>
-    <tableColumn id="12" name="VS.Gmm_failGprsAttachRadioStatus_G"/>
-    <tableColumn id="13" name="VS.Gmm_rejGprsAttachIllegalME_G"/>
-    <tableColumn id="14" name="VS.Gmm_GprsRejAttachAccRestrData_G"/>
-    <tableColumn id="15" name="VS.Gmm_failGprsAttachTimeout_G"/>
-    <tableColumn id="16" name="VS.Gmm_rejGprsAttachImsiAttachedSgsnInternal_G"/>
-    <tableColumn id="17" name="VS.Gmm_rejGprsAttachImsiAttachedNetworkFailure_G"/>
-    <tableColumn id="18" name="VS.Gmm_rejGprsAttachImsiAttachedProtocolError_G"/>
-    <tableColumn id="19" name="VS.Gmm_rejGprsAttachGprsAndNonGprsServiceNotAllowed_G"/>
-    <tableColumn id="20" name="VS.Gmm_attGprsDetachSgsn_G"/>
-    <tableColumn id="21" name="VS.Sm_attActPDPCtxMSPerSgsn_G"/>
-    <tableColumn id="22" name="VS.Sm_succActPDPCtxMSPerSgsn_G"/>
-    <tableColumn id="23" name="VS.Sm_RejActPDPCtxAuthenticationFailed_G"/>
-    <tableColumn id="24" name="VS.Sm_RejActPDPCtxNoResources_G"/>
-    <tableColumn id="25" name="VS.Sm_RejActPDPCtxByGgsn_G"/>
-    <tableColumn id="35" name="VS.Sm_AveNbrActivePDPCtx_G"/>
-    <tableColumn id="30" name="VS.Bssgp_UpUnitDataKBytesRcv"/>
-    <tableColumn id="31" name="VS.Bssgp_DownUnitDataKBytesSent"/>
-    <tableColumn id="26" name="VS.Sm_RejActPDPCtxUnspecified_G"/>
-    <tableColumn id="38" name="VS.Sm_RejActPDPCtxOptionNotSupported_G"/>
-    <tableColumn id="37" name="VS.Sm_RejActPDPCtxOptionNotSubscribed_G"/>
-    <tableColumn id="36" name="VS.Sm_RejActPDPCtxOptionOutOfOrder_G"/>
-    <tableColumn id="34" name="Column1"/>
-    <tableColumn id="27" name="Attach Rate" dataDxfId="15">
-      <calculatedColumnFormula>(F2+J2+K2+L2)/E2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="28" name="Attach Rate (netw failures NOT included)" dataDxfId="14">
-      <calculatedColumnFormula>(F2+I2+J2+K2+L2)/E2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="29" name="PDP Context Activation Rate" dataDxfId="13">
-      <calculatedColumnFormula>(V2+W2+X2+Y2)/U2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="32" name="Gb DL Mbps" dataDxfId="12">
-      <calculatedColumnFormula>AB2*8/1024/900</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="33" name="Gb UL Mbps" dataDxfId="11">
-      <calculatedColumnFormula>AA2*8/1024/900</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:AR2" insertRow="1" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A1:AR2"/>
-  <tableColumns count="44">
-    <tableColumn id="1" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" name="Time" dataDxfId="8"/>
-    <tableColumn id="3" name="VS.Gmm_AveNbrOfAttachedSub_U"/>
-    <tableColumn id="4" name="VS.Gmm_MaxNbrOfAttachedSub_U"/>
-    <tableColumn id="5" name="VS.Gmm_attGprsAttach_U"/>
-    <tableColumn id="6" name="VS.Gmm_succGprsAttach_U"/>
-    <tableColumn id="7" name="VS.Gmm_rejGprsAttachSgsnInternal_U"/>
-    <tableColumn id="8" name="VS.Gmm_rejGprsAttachProtocolError_U"/>
-    <tableColumn id="9" name="VS.Gmm_rejGprsAttachNetworkFailure_U"/>
-    <tableColumn id="10" name="VS.Gmm_failGprsAttachTimeout_U"/>
-    <tableColumn id="11" name="VS.Gmm_rejGprsAttachNotAllowed_U"/>
-    <tableColumn id="12" name="VS.Gmm_rejGprsAttachIllegalME_U"/>
-    <tableColumn id="13" name="VS.Gmm_GprsRejAttachAccRestrData_U"/>
-    <tableColumn id="14" name="VS.Gmm_rejGprsAttachImsiAttachedSgsnInternal_U"/>
-    <tableColumn id="15" name="VS.Gmm_rejGprsAttachImsiAttachedNetworkFailure_U"/>
-    <tableColumn id="16" name="VS.Gmm_rejGprsAttachImsiAttachedProtocolError_U"/>
-    <tableColumn id="17" name="VS.Gmm_rejGprsAttachGprsAndNonGprsServiceNotAllowed_U"/>
-    <tableColumn id="18" name="VS.Gmm_attGprsDetachSgsn_U"/>
-    <tableColumn id="19" name="VS.Sm_AveNbrActivePDPCtx_U"/>
-    <tableColumn id="20" name="VS.Sm_InstNbrActivePDPCtx_U"/>
-    <tableColumn id="21" name="VS.Sm_MaxNbrActivePDPCtx_U"/>
-    <tableColumn id="22" name="VS.Sm_attActPDPCtxMSPerSgsn_U"/>
-    <tableColumn id="23" name="VS.Sm_succActPDPCtxMSPerSgsn_U"/>
-    <tableColumn id="24" name="VS.Sm_RejActPDPCtxAuthenticationFailed_U"/>
-    <tableColumn id="25" name="VS.Sm_RejActPDPCtxNoResources_U"/>
-    <tableColumn id="26" name="VS.Sm_RejActPDPCtxByGgsn_U"/>
-    <tableColumn id="27" name="VS.Sm_RejActPDPCtxUnspecified_U"/>
-    <tableColumn id="28" name="VS.Sm_RejActPDPCtxOptionNotSubscribed_U"/>
-    <tableColumn id="29" name="VS.Sm_RejActPDPCtxOptionNotSupported_U"/>
-    <tableColumn id="30" name="VS.Sm_RejActPDPCtxProtocolError_U"/>
-    <tableColumn id="31" name="VS.Sm_RejActPDPCtxOptionOutOfOrder_U"/>
-    <tableColumn id="32" name="VS.Sm_RejActPDPCtxMessageDecoding_U"/>
-    <tableColumn id="33" name="VS.Gtpu_DownKBytesSent"/>
-    <tableColumn id="34" name="VS.Gtpu_DownKBytesRcv"/>
-    <tableColumn id="43" name="VS.Gmm_rejGprsAttachMSIdentification_U"/>
-    <tableColumn id="42" name="VS.Gmm_rejGprsAttachSubscriptionOptions_U"/>
-    <tableColumn id="41" name="VS.Gmm_failGprsAttachCpuLoad_U"/>
-    <tableColumn id="35" name="Column1" dataDxfId="7"/>
-    <tableColumn id="36" name="Attach Rate 3G" dataDxfId="6">
-      <calculatedColumnFormula>(F2+K2 + I2 + L2 + Q2+ AI2 + AJ2)/(F2+K2 + I2 + L2 + Q2 + G2 + H2 + J2 + AK2)%</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="44" name="Attach Rate 3G (customer)" dataDxfId="5">
-      <calculatedColumnFormula>(K2+F2)/E2%</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="37" name="PDP Rate 3G" dataDxfId="4">
-      <calculatedColumnFormula>(W2+AC2+AB2)/(AC2+AB2+W2+Y2+X2+Z2+AA2+AD2+AE2+AF2)%</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="38" name="3G Ul" dataDxfId="3">
-      <calculatedColumnFormula>ROUND(AG2*8/1024/900,2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="39" name="3G Dl" dataDxfId="2">
-      <calculatedColumnFormula>ROUND(AH2*8/1024/900,2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="40" name="3G UL+DL" dataDxfId="1">
-      <calculatedColumnFormula>AP2+AQ2</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5841,10 +5641,10 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="10:13" ht="23" x14ac:dyDescent="0.5">
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="7"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5860,8 +5660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5894,184 +5694,129 @@
     <col min="37" max="38" width="3.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="2" customFormat="1" ht="250.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:38" s="1" customFormat="1" ht="250.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="6"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="0" priority="27" operator="greaterThan">
-      <formula>346000</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI2:AJ2">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="num" val="0.7"/>
-        <cfvo type="num" val="0.85"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W2">
-    <cfRule type="colorScale" priority="267">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="num" val="30"/>
-        <color theme="0"/>
-        <color theme="3" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y2">
-    <cfRule type="colorScale" priority="268">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="num" val="30"/>
-        <color theme="0"/>
-        <color theme="6" tint="0.39997558519241921"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2">
-    <cfRule type="colorScale" priority="269">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="num" val="10"/>
-        <color theme="0"/>
-        <color theme="5" tint="0.39997558519241921"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -6079,8 +5824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AJ11" sqref="AJ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6103,156 +5848,146 @@
     <col min="44" max="44" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="269.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:44" ht="269.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AL1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AM1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AP1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AR1" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="6"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="8"/>
-      <c r="AQ2" s="8"/>
-      <c r="AR2" s="8"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>